<commit_message>
ExcelCompare implementatiopn of compareSheet(), compareRow()...
</commit_message>
<xml_diff>
--- a/src/excelA.xlsx
+++ b/src/excelA.xlsx
@@ -125,10 +125,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -149,6 +149,146 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>